<commit_message>
Entrega Lab4- Final Gssanchez
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\EDA\LabSorts-S04-G13\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2EB8E8-EEAF-4C8C-A661-9CDBD604BA76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,17 @@
     <sheet name="Graf Selection Sort" sheetId="10" r:id="rId5"/>
     <sheet name="Graf Shell Sort" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <r>
       <t>T</t>
@@ -79,12 +70,15 @@
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
   </si>
+  <si>
+    <t>106,.17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +99,24 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Dex-regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Dex"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -144,11 +156,21 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -362,31 +384,6 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -459,7 +456,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +523,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +610,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -664,34 +661,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>681.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2736.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>10986.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>47835.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>195440.73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>783566.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +766,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -832,34 +817,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>790.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3136.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>13491.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>54526.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>223217.96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>862018.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,7 +921,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -996,37 +969,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>37.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>78.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>182.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>453.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2546.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>6194.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>14976.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>37209.300000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,7 +1096,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1134,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1218,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1256,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1298,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1335,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1374,7 +1344,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1411,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1528,7 +1498,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1696,7 +1666,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1863,7 +1833,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2041,7 +2011,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +2049,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +2133,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +2171,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2250,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2289,7 +2259,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2356,7 +2326,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,7 +2414,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2495,34 +2465,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>681.86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2736.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>10986.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>47835.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>195440.73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>783566.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,7 +2570,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2790,7 +2748,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2865,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2903,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2945,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +2982,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3033,7 +2991,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3095,7 +3053,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +3141,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3234,34 +3192,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>790.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3136.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>13491.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>54526.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>223217.96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>862018.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,7 +3297,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3529,7 +3475,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3513,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3592,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3630,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3672,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3709,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3772,7 +3718,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3834,7 +3780,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,7 +3868,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3970,37 +3916,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>37.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>78.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>182.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>453.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2546.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>6194.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>14976.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>37209.300000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,7 +4033,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4268,7 +4211,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4249,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,11 +4328,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4423,7 +4366,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4408,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4445,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +7229,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7240,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="83" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7251,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="83" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +7262,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="83" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7273,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7284,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290892" cy="6059277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7317,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290892" cy="6059277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7350,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290892" cy="6059277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7383,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9290892" cy="6059277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7416,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290892" cy="6059277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7503,13 +7446,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Shell Sort [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7529,7 +7472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7825,21 +7768,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,164 +7796,130 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>681.86</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>790.72</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="D2" s="5">
+        <v>37.18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>2736.67</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>3136.76</v>
       </c>
-      <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+      <c r="D3" s="6">
+        <v>78.650000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>10986.6</v>
       </c>
       <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>13491.95</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+      <c r="D4" s="6">
+        <v>182.59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>47835.46</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>54526.17</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="D5" s="7">
+        <v>453.79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>195440.73</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>223217.96</v>
       </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4">
-        <v>60</v>
+        <v>783566.2</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>862018.54</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+      <c r="D7" s="7">
+        <v>2546.1999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="7">
+        <v>6194.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7">
+        <v>14976.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7">
+        <v>37209.300000000003</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
+      <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8023,8 +7932,9 @@
       <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -8038,7 +7948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -8053,7 +7963,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -8061,15 +7971,15 @@
         <v>70</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
+        <f t="shared" ref="C17:C24" si="0">C16+C15</f>
         <v>6</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
+        <f t="shared" ref="D17:D24" si="1">D16+10</f>
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -8077,15 +7987,15 @@
         <v>80</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
@@ -8093,15 +8003,15 @@
         <v>90</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
@@ -8109,15 +8019,15 @@
         <v>100</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
@@ -8125,15 +8035,15 @@
         <v>110</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
@@ -8141,15 +8051,15 @@
         <v>120</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
@@ -8157,15 +8067,15 @@
         <v>130</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
@@ -8173,11 +8083,11 @@
         <v>140</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
     </row>
@@ -8200,6 +8110,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -8410,12 +8326,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
@@ -8425,6 +8335,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8441,13 +8360,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>